<commit_message>
:memo: Update codes and add figures
</commit_message>
<xml_diff>
--- a/Sheets/METRICS.xlsx
+++ b/Sheets/METRICS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Github\2021-IEEE-IJCNN\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA2501-19D8-401B-8B79-7C6771CA050C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A4E9F8-F016-4EA7-B301-F22B1C10A70E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23040" yWindow="375" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>MAPE</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
     <t>1-step-ahead</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>14-steps-ahead</t>
+  </si>
+  <si>
+    <t>RMSPE</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -182,6 +182,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -198,29 +201,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -511,7 +492,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,12 +528,12 @@
         <v>7</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>11</v>
+      <c r="A2" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
@@ -581,26 +562,26 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="10">
         <v>8.2703423230209502E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="10">
         <v>8.9516926380510897E-2</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10">
         <v>0.15083636724712601</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="10">
         <v>0.16163773864841699</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="10">
         <v>0.15896531202925701</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="10">
         <v>0.16430397291148199</v>
       </c>
       <c r="I3" s="7">
@@ -609,36 +590,36 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="9">
-        <v>613.07388168343903</v>
+        <v>0.16773438337948901</v>
       </c>
       <c r="D4" s="9">
-        <v>650.09577745068998</v>
+        <v>0.20136626778904601</v>
       </c>
       <c r="E4" s="9">
-        <v>1484.3015582409</v>
+        <v>0.63274444040759303</v>
       </c>
       <c r="F4" s="9">
-        <v>1459.69498301098</v>
+        <v>0.54646621070986501</v>
       </c>
       <c r="G4" s="9">
-        <v>1390.45510306251</v>
+        <v>0.47860864967153699</v>
       </c>
       <c r="H4" s="9">
-        <v>1679.9044749539901</v>
+        <v>0.70633953489604595</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" si="0"/>
-        <v>613.07388168343903</v>
+        <v>0.16773438337948901</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>13</v>
+      <c r="A5" s="11" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>8</v>
@@ -667,26 +648,26 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="10">
         <v>0.177691160760024</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="10">
         <v>0.17537535964793899</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="10">
         <v>0.18443286907414599</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="10">
         <v>0.190978212003172</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="10">
         <v>0.19380398759173101</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="10">
         <v>0.19141343726110099</v>
       </c>
       <c r="I6" s="7">
@@ -695,36 +676,36 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" s="9">
-        <v>1406.6892101312501</v>
+        <v>0.31848817192849699</v>
       </c>
       <c r="D7" s="9">
-        <v>1307.453532539</v>
+        <v>0.28893970912988098</v>
       </c>
       <c r="E7" s="9">
-        <v>1666.3642392070001</v>
+        <v>0.65374187699785102</v>
       </c>
       <c r="F7" s="9">
-        <v>1805.1076686670101</v>
+        <v>0.75938662245705602</v>
       </c>
       <c r="G7" s="9">
-        <v>1878.30180771186</v>
+        <v>0.77674007543253898</v>
       </c>
       <c r="H7" s="9">
-        <v>1761.9816749208501</v>
+        <v>0.702262520077235</v>
       </c>
       <c r="I7" s="9">
         <f t="shared" si="0"/>
-        <v>1307.453532539</v>
+        <v>0.28893970912988098</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>14</v>
+      <c r="A8" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
@@ -753,26 +734,26 @@
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="10">
         <v>0.206572388029822</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="10">
         <v>0.19347306429474101</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="10">
         <v>0.18846898656630301</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="10">
         <v>0.210608824487131</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="10">
         <v>0.19669901506626</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="10">
         <v>0.21642079535091299</v>
       </c>
       <c r="I9" s="7">
@@ -781,31 +762,31 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9">
-        <v>1512.10561791334</v>
+        <v>0.33765680542097298</v>
       </c>
       <c r="D10" s="9">
-        <v>1429.4544971216999</v>
+        <v>0.30752593515346099</v>
       </c>
       <c r="E10" s="9">
-        <v>1704.5073320348699</v>
+        <v>0.65587084906632198</v>
       </c>
       <c r="F10" s="9">
-        <v>1875.32457221512</v>
+        <v>0.76186560473199405</v>
       </c>
       <c r="G10" s="9">
-        <v>1873.93694424928</v>
+        <v>0.77672510211081902</v>
       </c>
       <c r="H10" s="9">
-        <v>1857.7827748115401</v>
+        <v>0.70642851615069502</v>
       </c>
       <c r="I10" s="9">
         <f t="shared" si="0"/>
-        <v>1429.4544971216999</v>
+        <v>0.30752593515346099</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +796,7 @@
     <mergeCell ref="A8:A10"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:I10">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
:memo: Update codes and add new figures
</commit_message>
<xml_diff>
--- a/Sheets/METRICS.xlsx
+++ b/Sheets/METRICS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Github\2021-IEEE-IJCNN\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A4E9F8-F016-4EA7-B301-F22B1C10A70E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83909414-28A3-4B95-B1DE-70C3348407BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23040" yWindow="375" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-1095" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
   <si>
     <t>Forecasting Horizon</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>RMSPE</t>
+  </si>
+  <si>
+    <t>Menor</t>
+  </si>
+  <si>
+    <t>Maior</t>
+  </si>
+  <si>
+    <t>Improvement Perfomance Index</t>
   </si>
 </sst>
 </file>
@@ -155,7 +164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,6 +196,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -195,13 +207,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -489,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +546,7 @@
     <col min="10" max="16384" width="15.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -531,8 +575,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -561,8 +605,8 @@
         <v>470.264262417243</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
@@ -589,8 +633,8 @@
         <v>8.2703423230209502E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
@@ -617,8 +661,8 @@
         <v>0.16773438337948901</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -647,8 +691,8 @@
         <v>1039.3100213607199</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -675,8 +719,8 @@
         <v>0.17537535964793899</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
@@ -703,8 +747,8 @@
         <v>0.28893970912988098</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -733,8 +777,8 @@
         <v>1179.10313392387</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
@@ -761,8 +805,8 @@
         <v>0.18846898656630301</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
@@ -789,14 +833,312 @@
         <v>0.30752593515346099</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15">
+        <f>(C3-$C3)/C3</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="15">
+        <f>(D3-$C3)/D3</f>
+        <v>7.6114131994871437E-2</v>
+      </c>
+      <c r="E14" s="15">
+        <f>(E3-$C3)/E3</f>
+        <v>0.45170104040817577</v>
+      </c>
+      <c r="F14" s="15">
+        <f>(F3-$C3)/F3</f>
+        <v>0.4883408792911898</v>
+      </c>
+      <c r="G14" s="15">
+        <f>(G3-$C3)/G3</f>
+        <v>0.47973918225009854</v>
+      </c>
+      <c r="H14" s="15">
+        <f>(H3-$C3)/H3</f>
+        <v>0.4966438013354334</v>
+      </c>
+      <c r="J14" s="17">
+        <f>SMALL(C14:H14,2)</f>
+        <v>7.6114131994871437E-2</v>
+      </c>
+      <c r="K14" s="17">
+        <f>LARGE(C14:H14,1)</f>
+        <v>0.4966438013354334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="16">
+        <f>(C4-$C4)/C4</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="16">
+        <f>(D4-$C4)/D4</f>
+        <v>0.16701846232155532</v>
+      </c>
+      <c r="E15" s="16">
+        <f>(E4-$C4)/E4</f>
+        <v>0.73490974765192718</v>
+      </c>
+      <c r="F15" s="16">
+        <f>(F4-$C4)/F4</f>
+        <v>0.6930562583886013</v>
+      </c>
+      <c r="G15" s="16">
+        <f>(G4-$C4)/G4</f>
+        <v>0.64953750105727714</v>
+      </c>
+      <c r="H15" s="16">
+        <f>(H4-$C4)/H4</f>
+        <v>0.76253009340023004</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" ref="J15:J19" si="1">SMALL(C15:H15,2)</f>
+        <v>0.16701846232155532</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" ref="K15:K19" si="2">LARGE(C15:H15,1)</f>
+        <v>0.76253009340023004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="15">
+        <f>(C6-$D6)/C6</f>
+        <v>1.3032731072158152E-2</v>
+      </c>
+      <c r="D16" s="15">
+        <f>(D6-$D6)/D6</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="15">
+        <f>(E6-$D6)/E6</f>
+        <v>4.9110060867543576E-2</v>
+      </c>
+      <c r="F16" s="15">
+        <f>(F6-$D6)/F6</f>
+        <v>8.1699646213955854E-2</v>
+      </c>
+      <c r="G16" s="15">
+        <f>(G6-$D6)/G6</f>
+        <v>9.5089002929154953E-2</v>
+      </c>
+      <c r="H16" s="15">
+        <f>(H6-$D6)/H6</f>
+        <v>8.3787626629811637E-2</v>
+      </c>
+      <c r="J16" s="17">
+        <f t="shared" si="1"/>
+        <v>1.3032731072158152E-2</v>
+      </c>
+      <c r="K16" s="17">
+        <f t="shared" si="2"/>
+        <v>9.5089002929154953E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="16">
+        <f>(C7-$D7)/C7</f>
+        <v>9.2777268994623324E-2</v>
+      </c>
+      <c r="D17" s="16">
+        <f>(D7-$D7)/D7</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="16">
+        <f>(E7-$D7)/E7</f>
+        <v>0.55802172188086585</v>
+      </c>
+      <c r="F17" s="16">
+        <f>(F7-$D7)/F7</f>
+        <v>0.61950908722227227</v>
+      </c>
+      <c r="G17" s="16">
+        <f>(G7-$D7)/G7</f>
+        <v>0.62800978310668376</v>
+      </c>
+      <c r="H17" s="16">
+        <f>(H7-$D7)/H7</f>
+        <v>0.58855883537953391</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="1"/>
+        <v>9.2777268994623324E-2</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="2"/>
+        <v>0.62800978310668376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="15">
+        <f>(C9-$E9)/C9</f>
+        <v>8.7637082749440251E-2</v>
+      </c>
+      <c r="D18" s="15">
+        <f>(D9-$E9)/D9</f>
+        <v>2.5864467215005602E-2</v>
+      </c>
+      <c r="E18" s="15">
+        <f>(E9-$E9)/E9</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <f>(F9-$E9)/F9</f>
+        <v>0.1051230306932406</v>
+      </c>
+      <c r="G18" s="15">
+        <f>(G9-$E9)/G9</f>
+        <v>4.1840720438710011E-2</v>
+      </c>
+      <c r="H18" s="15">
+        <f>(H9-$E9)/H9</f>
+        <v>0.1291549120281526</v>
+      </c>
+      <c r="J18" s="17">
+        <f t="shared" si="1"/>
+        <v>2.5864467215005602E-2</v>
+      </c>
+      <c r="K18" s="17">
+        <f t="shared" si="2"/>
+        <v>0.1291549120281526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="16">
+        <f>(C10-$D10)/C10</f>
+        <v>8.9235193201411656E-2</v>
+      </c>
+      <c r="D19" s="16">
+        <f>(D10-$D10)/D10</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="16">
+        <f>(E10-$D10)/E10</f>
+        <v>0.53111815292409215</v>
+      </c>
+      <c r="F19" s="16">
+        <f>(F10-$D10)/F10</f>
+        <v>0.59635146508334469</v>
+      </c>
+      <c r="G19" s="16">
+        <f>(G10-$D10)/G10</f>
+        <v>0.60407364932878815</v>
+      </c>
+      <c r="H19" s="16">
+        <f>(H10-$D10)/H10</f>
+        <v>0.56467508300888059</v>
+      </c>
+      <c r="J19" s="17">
+        <f t="shared" si="1"/>
+        <v>8.9235193201411656E-2</v>
+      </c>
+      <c r="K19" s="17">
+        <f t="shared" si="2"/>
+        <v>0.60407364932878815</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J22" s="18">
+        <f>MIN(J14:K19)</f>
+        <v>1.3032731072158152E-2</v>
+      </c>
+      <c r="K22" s="18">
+        <f>MAX(J14:K19)</f>
+        <v>0.76253009340023004</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:I10">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C2:I11">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:H19">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
:memo: Add new figures and Update codes
</commit_message>
<xml_diff>
--- a/Sheets/METRICS.xlsx
+++ b/Sheets/METRICS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\Documents\Github\2021-IEEE-IJCNN\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83909414-28A3-4B95-B1DE-70C3348407BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13A4A96-D64A-459A-A9C5-CAB51F16C0A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1095" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha 1" sheetId="1" r:id="rId1"/>
@@ -199,35 +199,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -576,7 +576,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -606,7 +606,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
@@ -634,7 +634,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="20"/>
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
@@ -662,7 +662,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -692,7 +692,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -720,7 +720,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
@@ -748,7 +748,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -778,7 +778,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
@@ -806,7 +806,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
@@ -835,17 +835,17 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="18" t="s">
         <v>17</v>
       </c>
     </row>
@@ -882,245 +882,245 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="15">
-        <f>(C3-$C3)/C3</f>
+      <c r="C14" s="12">
+        <f t="shared" ref="C14:H15" si="1">(C3-$C3)/C3</f>
         <v>0</v>
       </c>
-      <c r="D14" s="15">
-        <f>(D3-$C3)/D3</f>
+      <c r="D14" s="12">
+        <f t="shared" si="1"/>
         <v>7.6114131994871437E-2</v>
       </c>
-      <c r="E14" s="15">
-        <f>(E3-$C3)/E3</f>
+      <c r="E14" s="12">
+        <f t="shared" si="1"/>
         <v>0.45170104040817577</v>
       </c>
-      <c r="F14" s="15">
-        <f>(F3-$C3)/F3</f>
+      <c r="F14" s="12">
+        <f t="shared" si="1"/>
         <v>0.4883408792911898</v>
       </c>
-      <c r="G14" s="15">
-        <f>(G3-$C3)/G3</f>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
         <v>0.47973918225009854</v>
       </c>
-      <c r="H14" s="15">
-        <f>(H3-$C3)/H3</f>
+      <c r="H14" s="12">
+        <f t="shared" si="1"/>
         <v>0.4966438013354334</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="14">
         <f>SMALL(C14:H14,2)</f>
         <v>7.6114131994871437E-2</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="14">
         <f>LARGE(C14:H14,1)</f>
         <v>0.4966438013354334</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="16">
-        <f>(C4-$C4)/C4</f>
+      <c r="C15" s="13">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D15" s="16">
-        <f>(D4-$C4)/D4</f>
+      <c r="D15" s="13">
+        <f t="shared" si="1"/>
         <v>0.16701846232155532</v>
       </c>
-      <c r="E15" s="16">
-        <f>(E4-$C4)/E4</f>
+      <c r="E15" s="13">
+        <f t="shared" si="1"/>
         <v>0.73490974765192718</v>
       </c>
-      <c r="F15" s="16">
-        <f>(F4-$C4)/F4</f>
+      <c r="F15" s="13">
+        <f t="shared" si="1"/>
         <v>0.6930562583886013</v>
       </c>
-      <c r="G15" s="16">
-        <f>(G4-$C4)/G4</f>
+      <c r="G15" s="13">
+        <f t="shared" si="1"/>
         <v>0.64953750105727714</v>
       </c>
-      <c r="H15" s="16">
-        <f>(H4-$C4)/H4</f>
+      <c r="H15" s="13">
+        <f t="shared" si="1"/>
         <v>0.76253009340023004</v>
       </c>
-      <c r="J15" s="17">
-        <f t="shared" ref="J15:J19" si="1">SMALL(C15:H15,2)</f>
+      <c r="J15" s="14">
+        <f t="shared" ref="J15:J19" si="2">SMALL(C15:H15,2)</f>
         <v>0.16701846232155532</v>
       </c>
-      <c r="K15" s="17">
-        <f t="shared" ref="K15:K19" si="2">LARGE(C15:H15,1)</f>
+      <c r="K15" s="14">
+        <f t="shared" ref="K15:K19" si="3">LARGE(C15:H15,1)</f>
         <v>0.76253009340023004</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="15">
-        <f>(C6-$D6)/C6</f>
+      <c r="C16" s="12">
+        <f t="shared" ref="C16:H17" si="4">(C6-$D6)/C6</f>
         <v>1.3032731072158152E-2</v>
       </c>
-      <c r="D16" s="15">
-        <f>(D6-$D6)/D6</f>
+      <c r="D16" s="12">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="15">
-        <f>(E6-$D6)/E6</f>
+      <c r="E16" s="12">
+        <f t="shared" si="4"/>
         <v>4.9110060867543576E-2</v>
       </c>
-      <c r="F16" s="15">
-        <f>(F6-$D6)/F6</f>
+      <c r="F16" s="12">
+        <f t="shared" si="4"/>
         <v>8.1699646213955854E-2</v>
       </c>
-      <c r="G16" s="15">
-        <f>(G6-$D6)/G6</f>
+      <c r="G16" s="12">
+        <f t="shared" si="4"/>
         <v>9.5089002929154953E-2</v>
       </c>
-      <c r="H16" s="15">
-        <f>(H6-$D6)/H6</f>
+      <c r="H16" s="12">
+        <f t="shared" si="4"/>
         <v>8.3787626629811637E-2</v>
       </c>
-      <c r="J16" s="17">
-        <f t="shared" si="1"/>
+      <c r="J16" s="14">
+        <f t="shared" si="2"/>
         <v>1.3032731072158152E-2</v>
       </c>
-      <c r="K16" s="17">
-        <f t="shared" si="2"/>
+      <c r="K16" s="14">
+        <f t="shared" si="3"/>
         <v>9.5089002929154953E-2</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="16">
-        <f>(C7-$D7)/C7</f>
+      <c r="C17" s="13">
+        <f t="shared" si="4"/>
         <v>9.2777268994623324E-2</v>
       </c>
-      <c r="D17" s="16">
-        <f>(D7-$D7)/D7</f>
+      <c r="D17" s="13">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E17" s="16">
-        <f>(E7-$D7)/E7</f>
+      <c r="E17" s="13">
+        <f t="shared" si="4"/>
         <v>0.55802172188086585</v>
       </c>
-      <c r="F17" s="16">
-        <f>(F7-$D7)/F7</f>
+      <c r="F17" s="13">
+        <f t="shared" si="4"/>
         <v>0.61950908722227227</v>
       </c>
-      <c r="G17" s="16">
-        <f>(G7-$D7)/G7</f>
+      <c r="G17" s="13">
+        <f t="shared" si="4"/>
         <v>0.62800978310668376</v>
       </c>
-      <c r="H17" s="16">
-        <f>(H7-$D7)/H7</f>
+      <c r="H17" s="13">
+        <f t="shared" si="4"/>
         <v>0.58855883537953391</v>
       </c>
-      <c r="J17" s="17">
-        <f t="shared" si="1"/>
+      <c r="J17" s="14">
+        <f t="shared" si="2"/>
         <v>9.2777268994623324E-2</v>
       </c>
-      <c r="K17" s="17">
-        <f t="shared" si="2"/>
+      <c r="K17" s="14">
+        <f t="shared" si="3"/>
         <v>0.62800978310668376</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="15">
-        <f>(C9-$E9)/C9</f>
+      <c r="C18" s="12">
+        <f t="shared" ref="C18:H18" si="5">(C9-$E9)/C9</f>
         <v>8.7637082749440251E-2</v>
       </c>
-      <c r="D18" s="15">
-        <f>(D9-$E9)/D9</f>
+      <c r="D18" s="12">
+        <f t="shared" si="5"/>
         <v>2.5864467215005602E-2</v>
       </c>
-      <c r="E18" s="15">
-        <f>(E9-$E9)/E9</f>
+      <c r="E18" s="12">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F18" s="15">
-        <f>(F9-$E9)/F9</f>
+      <c r="F18" s="12">
+        <f t="shared" si="5"/>
         <v>0.1051230306932406</v>
       </c>
-      <c r="G18" s="15">
-        <f>(G9-$E9)/G9</f>
+      <c r="G18" s="12">
+        <f t="shared" si="5"/>
         <v>4.1840720438710011E-2</v>
       </c>
-      <c r="H18" s="15">
-        <f>(H9-$E9)/H9</f>
+      <c r="H18" s="12">
+        <f t="shared" si="5"/>
         <v>0.1291549120281526</v>
       </c>
-      <c r="J18" s="17">
-        <f t="shared" si="1"/>
+      <c r="J18" s="14">
+        <f t="shared" si="2"/>
         <v>2.5864467215005602E-2</v>
       </c>
-      <c r="K18" s="17">
-        <f t="shared" si="2"/>
+      <c r="K18" s="14">
+        <f t="shared" si="3"/>
         <v>0.1291549120281526</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="16">
-        <f>(C10-$D10)/C10</f>
+      <c r="C19" s="13">
+        <f t="shared" ref="C19:H19" si="6">(C10-$D10)/C10</f>
         <v>8.9235193201411656E-2</v>
       </c>
-      <c r="D19" s="16">
-        <f>(D10-$D10)/D10</f>
+      <c r="D19" s="13">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E19" s="16">
-        <f>(E10-$D10)/E10</f>
+      <c r="E19" s="13">
+        <f t="shared" si="6"/>
         <v>0.53111815292409215</v>
       </c>
-      <c r="F19" s="16">
-        <f>(F10-$D10)/F10</f>
+      <c r="F19" s="13">
+        <f t="shared" si="6"/>
         <v>0.59635146508334469</v>
       </c>
-      <c r="G19" s="16">
-        <f>(G10-$D10)/G10</f>
+      <c r="G19" s="13">
+        <f t="shared" si="6"/>
         <v>0.60407364932878815</v>
       </c>
-      <c r="H19" s="16">
-        <f>(H10-$D10)/H10</f>
+      <c r="H19" s="13">
+        <f t="shared" si="6"/>
         <v>0.56467508300888059</v>
       </c>
-      <c r="J19" s="17">
-        <f t="shared" si="1"/>
+      <c r="J19" s="14">
+        <f t="shared" si="2"/>
         <v>8.9235193201411656E-2</v>
       </c>
-      <c r="K19" s="17">
-        <f t="shared" si="2"/>
+      <c r="K19" s="14">
+        <f t="shared" si="3"/>
         <v>0.60407364932878815</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J22" s="18">
+      <c r="J22" s="15">
         <f>MIN(J14:K19)</f>
         <v>1.3032731072158152E-2</v>
       </c>
-      <c r="K22" s="18">
+      <c r="K22" s="15">
         <f>MAX(J14:K19)</f>
         <v>0.76253009340023004</v>
       </c>

</xml_diff>